<commit_message>
adding into to `env`
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="143">
   <si>
     <t>plant stress</t>
   </si>
@@ -98,9 +98,6 @@
     <t>year_min</t>
   </si>
   <si>
-    <t>topography</t>
-  </si>
-  <si>
     <t>dim</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>dbi</t>
   </si>
   <si>
-    <t>The exact spectral range of sensor varies among satellites</t>
-  </si>
-  <si>
     <t>mean</t>
   </si>
   <si>
@@ -411,13 +405,61 @@
   </si>
   <si>
     <t>season_type</t>
+  </si>
+  <si>
+    <t>landforms</t>
+  </si>
+  <si>
+    <t>soils</t>
+  </si>
+  <si>
+    <t>ASRIS</t>
+  </si>
+  <si>
+    <t>phc</t>
+  </si>
+  <si>
+    <t>swm</t>
+  </si>
+  <si>
+    <t>san</t>
+  </si>
+  <si>
+    <t>surface weighted soil texture index</t>
+  </si>
+  <si>
+    <t>surface weighted soil pH</t>
+  </si>
+  <si>
+    <t>leached-calcareous-saline soils, soil chemistry</t>
+  </si>
+  <si>
+    <t>infiltration, soil water balance, soil structure, soil chemistry</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Geoscience Australia</t>
+  </si>
+  <si>
+    <t>WOfS</t>
+  </si>
+  <si>
+    <t>wfs</t>
+  </si>
+  <si>
+    <t>water observations from space</t>
+  </si>
+  <si>
+    <t>lc25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +471,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -451,10 +501,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -463,8 +514,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -743,11 +796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S53"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N34" sqref="N34:N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,13 +826,13 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>17</v>
@@ -788,13 +841,13 @@
         <v>21</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>23</v>
@@ -809,18 +862,18 @@
         <v>8</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -829,31 +882,31 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J2" s="7">
         <v>1950</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O2" t="s">
         <v>1</v>
@@ -864,10 +917,10 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -876,31 +929,31 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="7">
         <v>1950</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O3" t="s">
         <v>1</v>
@@ -911,10 +964,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -923,34 +976,34 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="7">
         <v>1950</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L4" t="s">
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O4" t="s">
         <v>0</v>
@@ -961,10 +1014,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -973,13 +1026,13 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -991,13 +1044,13 @@
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L5" t="s">
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O5" t="s">
         <v>7</v>
@@ -1005,10 +1058,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -1017,16 +1070,16 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
@@ -1035,22 +1088,22 @@
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L6" t="s">
         <v>14</v>
       </c>
       <c r="M6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -1059,16 +1112,16 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" t="s">
         <v>6</v>
@@ -1077,21 +1130,21 @@
         <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L7" t="s">
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -1100,16 +1153,16 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" t="s">
         <v>6</v>
@@ -1118,21 +1171,21 @@
         <v>6</v>
       </c>
       <c r="K8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L8" t="s">
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -1141,16 +1194,16 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" t="s">
         <v>6</v>
@@ -1159,21 +1212,21 @@
         <v>6</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L9" t="s">
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -1182,16 +1235,16 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
         <v>6</v>
@@ -1200,21 +1253,21 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L10" t="s">
         <v>14</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -1223,16 +1276,16 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" t="s">
         <v>6</v>
@@ -1241,21 +1294,21 @@
         <v>6</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
       </c>
       <c r="M11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -1264,16 +1317,16 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" t="s">
         <v>6</v>
@@ -1282,21 +1335,21 @@
         <v>6</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L12" t="s">
         <v>14</v>
       </c>
       <c r="M12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -1305,16 +1358,16 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I13" t="s">
         <v>6</v>
@@ -1323,1714 +1376,1786 @@
         <v>6</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L13" t="s">
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14">
         <v>1989</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L14" t="s">
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J15">
         <v>1989</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L15" t="s">
         <v>2</v>
       </c>
       <c r="M15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H16" t="s">
         <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J16">
         <v>1989</v>
       </c>
       <c r="K16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L16" t="s">
         <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H17" t="s">
         <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17">
         <v>1989</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" t="s">
         <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18">
         <v>1989</v>
       </c>
       <c r="K18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L18" t="s">
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19">
         <v>1989</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J20">
         <v>1989</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J21">
         <v>1989</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H22" t="s">
         <v>19</v>
       </c>
       <c r="I22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22">
         <v>1989</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J23">
         <v>1989</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J24">
         <v>1989</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J25">
         <v>1989</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H26" t="s">
         <v>20</v>
       </c>
       <c r="I26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J26">
         <v>1989</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H27" t="s">
         <v>19</v>
       </c>
       <c r="I27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J27">
         <v>1989</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J28">
         <v>1989</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" t="s">
         <v>56</v>
       </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" t="s">
-        <v>57</v>
-      </c>
       <c r="G29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J29">
         <v>1989</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" t="s">
         <v>56</v>
       </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" t="s">
-        <v>57</v>
-      </c>
       <c r="G30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J30">
         <v>1989</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" t="s">
         <v>56</v>
       </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" t="s">
-        <v>126</v>
-      </c>
-      <c r="E31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" t="s">
-        <v>57</v>
-      </c>
       <c r="G31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H31" t="s">
         <v>20</v>
       </c>
       <c r="I31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J31">
         <v>1989</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" t="s">
         <v>56</v>
       </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" t="s">
-        <v>57</v>
-      </c>
       <c r="G32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H32" t="s">
         <v>19</v>
       </c>
       <c r="I32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J32">
         <v>1989</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" t="s">
         <v>56</v>
       </c>
-      <c r="C33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" t="s">
-        <v>126</v>
-      </c>
-      <c r="E33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" t="s">
-        <v>57</v>
-      </c>
       <c r="G33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J33">
         <v>1989</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J34">
         <v>1989</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M34" t="s">
-        <v>85</v>
-      </c>
-      <c r="N34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
         <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J35">
         <v>1989</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M35" t="s">
-        <v>101</v>
-      </c>
-      <c r="N35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H36" t="s">
         <v>20</v>
       </c>
       <c r="I36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J36">
         <v>1989</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M36" t="s">
-        <v>86</v>
-      </c>
-      <c r="N36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H37" t="s">
         <v>19</v>
       </c>
       <c r="I37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J37">
         <v>1989</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M37" t="s">
-        <v>87</v>
-      </c>
-      <c r="N37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J38">
         <v>1989</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M38" t="s">
-        <v>109</v>
-      </c>
-      <c r="N38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F39">
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J39">
         <v>1989</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M39" t="s">
-        <v>88</v>
-      </c>
-      <c r="N39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F40">
         <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J40">
         <v>1989</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M40" t="s">
-        <v>102</v>
-      </c>
-      <c r="N40" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
         <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F41">
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H41" t="s">
         <v>20</v>
       </c>
       <c r="I41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J41">
         <v>1989</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M41" t="s">
-        <v>89</v>
-      </c>
-      <c r="N41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
         <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F42">
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H42" t="s">
         <v>19</v>
       </c>
       <c r="I42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J42">
         <v>1989</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M42" t="s">
-        <v>90</v>
-      </c>
-      <c r="N42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
         <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F43">
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J43">
         <v>1989</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M43" t="s">
-        <v>110</v>
-      </c>
-      <c r="N43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F44">
         <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H44" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J44">
         <v>1989</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M44" t="s">
-        <v>91</v>
-      </c>
-      <c r="N44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F45">
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J45">
         <v>1989</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M45" t="s">
-        <v>103</v>
-      </c>
-      <c r="N45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
         <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F46">
         <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H46" t="s">
         <v>20</v>
       </c>
       <c r="I46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J46">
         <v>1989</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M46" t="s">
-        <v>92</v>
-      </c>
-      <c r="N46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F47">
         <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H47" t="s">
         <v>19</v>
       </c>
       <c r="I47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J47">
         <v>1989</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M47" t="s">
-        <v>93</v>
-      </c>
-      <c r="N47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" t="s">
         <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F48">
         <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J48">
         <v>1989</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M48" t="s">
-        <v>111</v>
-      </c>
-      <c r="N48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" t="s">
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F49">
         <v>4</v>
       </c>
       <c r="G49" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J49">
         <v>1989</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M49" t="s">
-        <v>94</v>
-      </c>
-      <c r="N49" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
         <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F50">
         <v>4</v>
       </c>
       <c r="G50" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J50">
         <v>1989</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M50" t="s">
-        <v>104</v>
-      </c>
-      <c r="N50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51" t="s">
         <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F51">
         <v>4</v>
       </c>
       <c r="G51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H51" t="s">
         <v>20</v>
       </c>
       <c r="I51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J51">
         <v>1989</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M51" t="s">
-        <v>95</v>
-      </c>
-      <c r="N51" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
         <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F52">
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H52" t="s">
         <v>19</v>
       </c>
       <c r="I52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J52">
         <v>1989</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M52" t="s">
-        <v>96</v>
-      </c>
-      <c r="N52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53" t="s">
         <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F53">
         <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H53" t="s">
+        <v>35</v>
+      </c>
+      <c r="I53" t="s">
+        <v>37</v>
+      </c>
+      <c r="J53">
+        <v>1989</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L53" t="s">
+        <v>43</v>
+      </c>
+      <c r="M53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" t="s">
+        <v>128</v>
+      </c>
+      <c r="C54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" t="s">
+        <v>130</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
+        <v>116</v>
+      </c>
+      <c r="H54" t="s">
+        <v>131</v>
+      </c>
+      <c r="I54" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54">
+        <v>1000</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M54" t="s">
+        <v>134</v>
+      </c>
+      <c r="O54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" t="s">
+        <v>129</v>
+      </c>
+      <c r="E55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>116</v>
+      </c>
+      <c r="H55" t="s">
+        <v>131</v>
+      </c>
+      <c r="I55" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55" t="s">
+        <v>6</v>
+      </c>
+      <c r="K55">
+        <v>10000</v>
+      </c>
+      <c r="L55" t="s">
+        <v>2</v>
+      </c>
+      <c r="M55" t="s">
+        <v>133</v>
+      </c>
+      <c r="O55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" t="s">
+        <v>138</v>
+      </c>
+      <c r="D56" t="s">
+        <v>139</v>
+      </c>
+      <c r="E56" t="s">
+        <v>142</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
+        <v>116</v>
+      </c>
+      <c r="H56" t="s">
+        <v>140</v>
+      </c>
+      <c r="I56" t="s">
         <v>36</v>
       </c>
-      <c r="I53" t="s">
-        <v>38</v>
-      </c>
-      <c r="J53">
-        <v>1989</v>
-      </c>
-      <c r="K53" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L53" t="s">
-        <v>44</v>
-      </c>
-      <c r="M53" t="s">
-        <v>112</v>
-      </c>
-      <c r="N53" t="s">
-        <v>71</v>
-      </c>
+      <c r="J56">
+        <v>1987</v>
+      </c>
+      <c r="K56">
+        <v>10000</v>
+      </c>
+      <c r="L56" t="s">
+        <v>2</v>
+      </c>
+      <c r="M56" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D62" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
aligning `env` with raster names
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -359,12 +359,6 @@
     <t>Landsat near infrared sensor standard deviation</t>
   </si>
   <si>
-    <t>tem</t>
-  </si>
-  <si>
-    <t>pre</t>
-  </si>
-  <si>
     <t>ari</t>
   </si>
   <si>
@@ -416,15 +410,9 @@
     <t>ASRIS</t>
   </si>
   <si>
-    <t>phc</t>
-  </si>
-  <si>
     <t>swm</t>
   </si>
   <si>
-    <t>san</t>
-  </si>
-  <si>
     <t>surface weighted soil texture index</t>
   </si>
   <si>
@@ -453,6 +441,18 @@
   </si>
   <si>
     <t>lc25</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>ph</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>prec</t>
   </si>
 </sst>
 </file>
@@ -799,8 +799,8 @@
   <dimension ref="A1:S62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N34" sqref="N34:N53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,10 +829,10 @@
         <v>49</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>17</v>
@@ -841,13 +841,13 @@
         <v>21</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>23</v>
@@ -882,13 +882,13 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H2" t="s">
         <v>70</v>
@@ -929,13 +929,13 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
         <v>70</v>
@@ -976,13 +976,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
         <v>70</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
@@ -1026,13 +1026,13 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
@@ -1070,13 +1070,13 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
         <v>28</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
         <v>53</v>
@@ -1112,13 +1112,13 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>53</v>
@@ -1153,13 +1153,13 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
         <v>27</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
@@ -1194,13 +1194,13 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
         <v>32</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
         <v>53</v>
@@ -1235,13 +1235,13 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
         <v>53</v>
@@ -1276,13 +1276,13 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H11" t="s">
         <v>33</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
         <v>53</v>
@@ -1317,13 +1317,13 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
         <v>53</v>
@@ -1358,13 +1358,13 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H13" t="s">
         <v>30</v>
@@ -1396,7 +1396,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -1405,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H14" t="s">
         <v>70</v>
@@ -1437,7 +1437,7 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
@@ -1446,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H15" t="s">
         <v>31</v>
@@ -1478,7 +1478,7 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -1487,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H16" t="s">
         <v>20</v>
@@ -1519,7 +1519,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
@@ -1528,7 +1528,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H17" t="s">
         <v>19</v>
@@ -1560,7 +1560,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
@@ -1569,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H18" t="s">
         <v>35</v>
@@ -1601,7 +1601,7 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s">
         <v>24</v>
@@ -1610,7 +1610,7 @@
         <v>44</v>
       </c>
       <c r="G19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H19" t="s">
         <v>70</v>
@@ -1642,7 +1642,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
         <v>24</v>
@@ -1651,7 +1651,7 @@
         <v>44</v>
       </c>
       <c r="G20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H20" t="s">
         <v>31</v>
@@ -1683,7 +1683,7 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E21" t="s">
         <v>24</v>
@@ -1692,7 +1692,7 @@
         <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
@@ -1724,7 +1724,7 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
@@ -1733,7 +1733,7 @@
         <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H22" t="s">
         <v>19</v>
@@ -1765,7 +1765,7 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
         <v>24</v>
@@ -1774,7 +1774,7 @@
         <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H23" t="s">
         <v>35</v>
@@ -1806,7 +1806,7 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E24" t="s">
         <v>24</v>
@@ -1815,7 +1815,7 @@
         <v>45</v>
       </c>
       <c r="G24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H24" t="s">
         <v>70</v>
@@ -1847,7 +1847,7 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E25" t="s">
         <v>24</v>
@@ -1856,7 +1856,7 @@
         <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H25" t="s">
         <v>31</v>
@@ -1888,7 +1888,7 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
         <v>24</v>
@@ -1897,7 +1897,7 @@
         <v>45</v>
       </c>
       <c r="G26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H26" t="s">
         <v>20</v>
@@ -1929,7 +1929,7 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E27" t="s">
         <v>24</v>
@@ -1938,7 +1938,7 @@
         <v>45</v>
       </c>
       <c r="G27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H27" t="s">
         <v>19</v>
@@ -1970,7 +1970,7 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E28" t="s">
         <v>24</v>
@@ -1979,7 +1979,7 @@
         <v>45</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H28" t="s">
         <v>35</v>
@@ -2011,7 +2011,7 @@
         <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E29" t="s">
         <v>24</v>
@@ -2020,7 +2020,7 @@
         <v>56</v>
       </c>
       <c r="G29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H29" t="s">
         <v>70</v>
@@ -2052,7 +2052,7 @@
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E30" t="s">
         <v>24</v>
@@ -2061,7 +2061,7 @@
         <v>56</v>
       </c>
       <c r="G30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H30" t="s">
         <v>31</v>
@@ -2093,7 +2093,7 @@
         <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E31" t="s">
         <v>24</v>
@@ -2102,7 +2102,7 @@
         <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H31" t="s">
         <v>20</v>
@@ -2134,7 +2134,7 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E32" t="s">
         <v>24</v>
@@ -2143,7 +2143,7 @@
         <v>56</v>
       </c>
       <c r="G32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H32" t="s">
         <v>19</v>
@@ -2175,7 +2175,7 @@
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E33" t="s">
         <v>24</v>
@@ -2184,7 +2184,7 @@
         <v>56</v>
       </c>
       <c r="G33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H33" t="s">
         <v>35</v>
@@ -2216,7 +2216,7 @@
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E34" t="s">
         <v>69</v>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H34" t="s">
         <v>70</v>
@@ -2257,7 +2257,7 @@
         <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E35" t="s">
         <v>69</v>
@@ -2266,7 +2266,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H35" t="s">
         <v>31</v>
@@ -2298,7 +2298,7 @@
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E36" t="s">
         <v>69</v>
@@ -2307,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H36" t="s">
         <v>20</v>
@@ -2339,7 +2339,7 @@
         <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E37" t="s">
         <v>69</v>
@@ -2348,7 +2348,7 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H37" t="s">
         <v>19</v>
@@ -2380,7 +2380,7 @@
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E38" t="s">
         <v>69</v>
@@ -2389,7 +2389,7 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H38" t="s">
         <v>35</v>
@@ -2421,7 +2421,7 @@
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E39" t="s">
         <v>69</v>
@@ -2430,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H39" t="s">
         <v>70</v>
@@ -2462,7 +2462,7 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
         <v>69</v>
@@ -2471,7 +2471,7 @@
         <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H40" t="s">
         <v>31</v>
@@ -2503,7 +2503,7 @@
         <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E41" t="s">
         <v>69</v>
@@ -2512,7 +2512,7 @@
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H41" t="s">
         <v>20</v>
@@ -2544,7 +2544,7 @@
         <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E42" t="s">
         <v>69</v>
@@ -2553,7 +2553,7 @@
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H42" t="s">
         <v>19</v>
@@ -2585,7 +2585,7 @@
         <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
         <v>69</v>
@@ -2594,7 +2594,7 @@
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H43" t="s">
         <v>35</v>
@@ -2626,7 +2626,7 @@
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E44" t="s">
         <v>69</v>
@@ -2635,7 +2635,7 @@
         <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H44" t="s">
         <v>70</v>
@@ -2667,7 +2667,7 @@
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E45" t="s">
         <v>69</v>
@@ -2676,7 +2676,7 @@
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H45" t="s">
         <v>31</v>
@@ -2708,7 +2708,7 @@
         <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E46" t="s">
         <v>69</v>
@@ -2717,7 +2717,7 @@
         <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H46" t="s">
         <v>20</v>
@@ -2749,7 +2749,7 @@
         <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E47" t="s">
         <v>69</v>
@@ -2758,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H47" t="s">
         <v>19</v>
@@ -2790,7 +2790,7 @@
         <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E48" t="s">
         <v>69</v>
@@ -2799,7 +2799,7 @@
         <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H48" t="s">
         <v>35</v>
@@ -2831,7 +2831,7 @@
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E49" t="s">
         <v>69</v>
@@ -2840,7 +2840,7 @@
         <v>4</v>
       </c>
       <c r="G49" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H49" t="s">
         <v>70</v>
@@ -2872,7 +2872,7 @@
         <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E50" t="s">
         <v>69</v>
@@ -2881,7 +2881,7 @@
         <v>4</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H50" t="s">
         <v>31</v>
@@ -2913,7 +2913,7 @@
         <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E51" t="s">
         <v>69</v>
@@ -2922,7 +2922,7 @@
         <v>4</v>
       </c>
       <c r="G51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H51" t="s">
         <v>20</v>
@@ -2954,7 +2954,7 @@
         <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E52" t="s">
         <v>69</v>
@@ -2963,7 +2963,7 @@
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H52" t="s">
         <v>19</v>
@@ -2995,7 +2995,7 @@
         <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E53" t="s">
         <v>69</v>
@@ -3004,7 +3004,7 @@
         <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H53" t="s">
         <v>35</v>
@@ -3027,28 +3027,28 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" t="s">
         <v>127</v>
       </c>
-      <c r="B54" t="s">
-        <v>128</v>
-      </c>
-      <c r="C54" t="s">
-        <v>129</v>
-      </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E54" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="F54">
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H54" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I54" t="s">
         <v>6</v>
@@ -3063,36 +3063,36 @@
         <v>6</v>
       </c>
       <c r="M54" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O54" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" t="s">
         <v>127</v>
       </c>
-      <c r="B55" t="s">
-        <v>128</v>
-      </c>
-      <c r="C55" t="s">
-        <v>129</v>
-      </c>
       <c r="D55" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E55" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H55" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I55" t="s">
         <v>6</v>
@@ -3107,36 +3107,36 @@
         <v>2</v>
       </c>
       <c r="M55" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O55" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D56" t="s">
+        <v>135</v>
+      </c>
+      <c r="E56" t="s">
         <v>138</v>
-      </c>
-      <c r="D56" t="s">
-        <v>139</v>
-      </c>
-      <c r="E56" t="s">
-        <v>142</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H56" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I56" t="s">
         <v>36</v>
@@ -3151,7 +3151,7 @@
         <v>2</v>
       </c>
       <c r="M56" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
aligning `env` with `prep_auscover`
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -50,9 +50,6 @@
     <t>helps with coastal shrubland</t>
   </si>
   <si>
-    <t>desc</t>
-  </si>
-  <si>
     <t>group</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>AusCover</t>
   </si>
   <si>
-    <t>prod</t>
-  </si>
-  <si>
     <t>dist</t>
   </si>
   <si>
@@ -453,6 +447,12 @@
   </si>
   <si>
     <t>median</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,90 +823,90 @@
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J2" s="7">
         <v>1950</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O2" t="s">
         <v>1</v>
@@ -917,43 +917,43 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J3" s="7">
         <v>1950</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O3" t="s">
         <v>1</v>
@@ -964,46 +964,46 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J4" s="7">
         <v>1950</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L4" t="s">
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O4" t="s">
         <v>0</v>
@@ -1014,28 +1014,28 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
         <v>6</v>
@@ -1044,13 +1044,13 @@
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L5" t="s">
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O5" t="s">
         <v>7</v>
@@ -1058,28 +1058,28 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
@@ -1088,40 +1088,40 @@
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
         <v>6</v>
@@ -1130,39 +1130,39 @@
         <v>6</v>
       </c>
       <c r="K7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
         <v>6</v>
@@ -1171,39 +1171,39 @@
         <v>6</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I9" t="s">
         <v>6</v>
@@ -1212,39 +1212,39 @@
         <v>6</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L9" t="s">
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
         <v>6</v>
@@ -1253,39 +1253,39 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I11" t="s">
         <v>6</v>
@@ -1294,39 +1294,39 @@
         <v>6</v>
       </c>
       <c r="K11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I12" t="s">
         <v>6</v>
@@ -1335,39 +1335,39 @@
         <v>6</v>
       </c>
       <c r="K12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I13" t="s">
         <v>6</v>
@@ -1376,1679 +1376,1679 @@
         <v>6</v>
       </c>
       <c r="K13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L13" t="s">
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14">
+        <v>1989</v>
+      </c>
+      <c r="K14" t="s">
         <v>36</v>
-      </c>
-      <c r="J14">
-        <v>1989</v>
-      </c>
-      <c r="K14" t="s">
-        <v>38</v>
       </c>
       <c r="L14" t="s">
         <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15">
+        <v>1989</v>
+      </c>
+      <c r="K15" t="s">
         <v>36</v>
-      </c>
-      <c r="J15">
-        <v>1989</v>
-      </c>
-      <c r="K15" t="s">
-        <v>38</v>
       </c>
       <c r="L15" t="s">
         <v>2</v>
       </c>
       <c r="M15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16">
+        <v>1989</v>
+      </c>
+      <c r="K16" t="s">
         <v>36</v>
-      </c>
-      <c r="J16">
-        <v>1989</v>
-      </c>
-      <c r="K16" t="s">
-        <v>38</v>
       </c>
       <c r="L16" t="s">
         <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17">
+        <v>1989</v>
+      </c>
+      <c r="K17" t="s">
         <v>36</v>
-      </c>
-      <c r="J17">
-        <v>1989</v>
-      </c>
-      <c r="K17" t="s">
-        <v>38</v>
       </c>
       <c r="L17" t="s">
         <v>2</v>
       </c>
       <c r="M17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18">
+        <v>1989</v>
+      </c>
+      <c r="K18" t="s">
         <v>36</v>
-      </c>
-      <c r="J18">
-        <v>1989</v>
-      </c>
-      <c r="K18" t="s">
-        <v>38</v>
       </c>
       <c r="L18" t="s">
         <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J19">
         <v>1989</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J20">
         <v>1989</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J21">
         <v>1989</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J22">
         <v>1989</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J23">
         <v>1989</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J24">
         <v>1989</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J25">
         <v>1989</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J26">
         <v>1989</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J27">
         <v>1989</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J28">
         <v>1989</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J29">
         <v>1989</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J30">
         <v>1989</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J31">
         <v>1989</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J32">
         <v>1989</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J33">
         <v>1989</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J34">
         <v>1989</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J35">
         <v>1989</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J36">
         <v>1989</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J37">
         <v>1989</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J38">
         <v>1989</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F39">
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J39">
         <v>1989</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E40" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F40">
         <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H40" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J40">
         <v>1989</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F41">
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J41">
         <v>1989</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F42">
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H42" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J42">
         <v>1989</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F43">
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H43" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J43">
         <v>1989</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F44">
         <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I44" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J44">
         <v>1989</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F45">
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J45">
         <v>1989</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E46" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F46">
         <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J46">
         <v>1989</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L46" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E47" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F47">
         <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J47">
         <v>1989</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F48">
         <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H48" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J48">
         <v>1989</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E49" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F49">
         <v>4</v>
       </c>
       <c r="G49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J49">
         <v>1989</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F50">
         <v>4</v>
       </c>
       <c r="G50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H50" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J50">
         <v>1989</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E51" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F51">
         <v>4</v>
       </c>
       <c r="G51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H51" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I51" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J51">
         <v>1989</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M51" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F52">
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H52" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I52" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J52">
         <v>1989</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L52" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M52" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E53" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F53">
         <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J53">
         <v>1989</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" t="s">
         <v>124</v>
       </c>
-      <c r="B54" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" t="s">
-        <v>126</v>
-      </c>
       <c r="D54" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F54">
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H54" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I54" t="s">
         <v>6</v>
@@ -3063,36 +3063,36 @@
         <v>6</v>
       </c>
       <c r="M54" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="O54" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" t="s">
         <v>124</v>
       </c>
-      <c r="B55" t="s">
-        <v>125</v>
-      </c>
-      <c r="C55" t="s">
-        <v>126</v>
-      </c>
       <c r="D55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I55" t="s">
         <v>6</v>
@@ -3107,39 +3107,39 @@
         <v>2</v>
       </c>
       <c r="M55" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="O55" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" t="s">
         <v>132</v>
       </c>
-      <c r="C56" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56" t="s">
-        <v>134</v>
-      </c>
       <c r="E56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I56" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J56">
         <v>1987</v>
@@ -3151,7 +3151,7 @@
         <v>2</v>
       </c>
       <c r="M56" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
product/process alignment with AusCover definitions
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -410,13 +410,13 @@
     <t>median</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
     <t>static</t>
+  </si>
+  <si>
+    <t>function</t>
   </si>
 </sst>
 </file>
@@ -764,7 +764,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,9 +773,9 @@
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -800,16 +800,16 @@
         <v>103</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>102</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>108</v>
@@ -824,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
updating units in `env`
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="149">
   <si>
     <t>plant stress</t>
   </si>
@@ -239,42 +239,6 @@
     <t>non-green vegetation cover max</t>
   </si>
   <si>
-    <t>Landsat blue sensor mean</t>
-  </si>
-  <si>
-    <t>Landsat blue sensor min</t>
-  </si>
-  <si>
-    <t>Landsat blue sensor max</t>
-  </si>
-  <si>
-    <t>Landsat green sensor mean</t>
-  </si>
-  <si>
-    <t>Landsat green sensor min</t>
-  </si>
-  <si>
-    <t>Landsat green sensor max</t>
-  </si>
-  <si>
-    <t>Landsat red sensor mean</t>
-  </si>
-  <si>
-    <t>Landsat red sensor min</t>
-  </si>
-  <si>
-    <t>Landsat red sensor max</t>
-  </si>
-  <si>
-    <t>Landsat near infrared sensor mean</t>
-  </si>
-  <si>
-    <t>Landsat near infrared sensor min</t>
-  </si>
-  <si>
-    <t>Landsat near infrared sensor max</t>
-  </si>
-  <si>
     <t>persistent green cover median</t>
   </si>
   <si>
@@ -287,18 +251,6 @@
     <t>non-green vegetation cover median</t>
   </si>
   <si>
-    <t>Landsat blue sensor median</t>
-  </si>
-  <si>
-    <t>Landsat green sensor median</t>
-  </si>
-  <si>
-    <t>Landsat red sensor median</t>
-  </si>
-  <si>
-    <t>Landsat near infrared sensor median</t>
-  </si>
-  <si>
     <t>persistent green cover standard deviation</t>
   </si>
   <si>
@@ -311,18 +263,6 @@
     <t>non-green vegetation cover standard deviation</t>
   </si>
   <si>
-    <t>Landsat blue sensor standard deviation</t>
-  </si>
-  <si>
-    <t>Landsat green sensor standard deviation</t>
-  </si>
-  <si>
-    <t>Landsat red sensor standard deviation</t>
-  </si>
-  <si>
-    <t>Landsat near infrared sensor standard deviation</t>
-  </si>
-  <si>
     <t>ari</t>
   </si>
   <si>
@@ -417,13 +357,138 @@
   </si>
   <si>
     <t>method</t>
+  </si>
+  <si>
+    <t>blue sensor max</t>
+  </si>
+  <si>
+    <t>blue sensor mean</t>
+  </si>
+  <si>
+    <t>blue sensor median</t>
+  </si>
+  <si>
+    <t>blue sensor min</t>
+  </si>
+  <si>
+    <t>blue sensor standard deviation</t>
+  </si>
+  <si>
+    <t>green sensor max</t>
+  </si>
+  <si>
+    <t>green sensor mean</t>
+  </si>
+  <si>
+    <t>green sensor median</t>
+  </si>
+  <si>
+    <t>green sensor min</t>
+  </si>
+  <si>
+    <t>green sensor standard deviation</t>
+  </si>
+  <si>
+    <t>red sensor max</t>
+  </si>
+  <si>
+    <t>red sensor mean</t>
+  </si>
+  <si>
+    <t>red sensor median</t>
+  </si>
+  <si>
+    <t>red sensor min</t>
+  </si>
+  <si>
+    <t>red sensor standard deviation</t>
+  </si>
+  <si>
+    <t>near infrared sensor max</t>
+  </si>
+  <si>
+    <t>near infrared sensor mean</t>
+  </si>
+  <si>
+    <t>near infrared sensor median</t>
+  </si>
+  <si>
+    <t>near infrared sensor min</t>
+  </si>
+  <si>
+    <t>near infrared sensor standard deviation</t>
+  </si>
+  <si>
+    <t>short-wave infrared 1 sensor mean</t>
+  </si>
+  <si>
+    <t>short-wave infrared 1 sensor median</t>
+  </si>
+  <si>
+    <t>short-wave infrared 1 sensor min</t>
+  </si>
+  <si>
+    <t>short-wave infrared 1 sensor standard deviation</t>
+  </si>
+  <si>
+    <t>short-wave infrared 1 sensor max</t>
+  </si>
+  <si>
+    <t>short-wave infrared 2 sensor max</t>
+  </si>
+  <si>
+    <t>short-wave infrared 2 sensor mean</t>
+  </si>
+  <si>
+    <t>short-wave infrared 2 sensor median</t>
+  </si>
+  <si>
+    <t>short-wave infrared 2 sensor min</t>
+  </si>
+  <si>
+    <t>short-wave infrared 2 sensor standard deviation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.11-2.29 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µm</t>
+    </r>
+  </si>
+  <si>
+    <t>1.57-1.65 µm</t>
+  </si>
+  <si>
+    <t>0.85-0.88 µm</t>
+  </si>
+  <si>
+    <t>0.64-0.67 µm</t>
+  </si>
+  <si>
+    <t>0.53-0.59 µm</t>
+  </si>
+  <si>
+    <t>0.45-0.51 µm</t>
+  </si>
+  <si>
+    <t>0.43-0.45 µm</t>
+  </si>
+  <si>
+    <t>µm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,6 +511,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -763,8 +834,8 @@
   <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,25 +865,25 @@
         <v>38</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>20</v>
@@ -824,7 +895,7 @@
         <v>2</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>35</v>
@@ -835,25 +906,25 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -871,10 +942,10 @@
         <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="O2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="2"/>
@@ -882,25 +953,25 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -918,10 +989,10 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="O3" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="2"/>
@@ -929,7 +1000,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -941,7 +1012,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -976,7 +1047,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -988,7 +1059,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1017,7 +1088,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -1029,7 +1100,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1059,7 +1130,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1071,7 +1142,7 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1100,7 +1171,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1112,7 +1183,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1141,7 +1212,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
@@ -1153,7 +1224,7 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1182,7 +1253,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -1194,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1223,7 +1294,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
@@ -1235,7 +1306,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1264,7 +1335,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
@@ -1276,7 +1347,7 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1314,7 +1385,7 @@
         <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
         <v>21</v>
@@ -1355,7 +1426,7 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
@@ -1396,7 +1467,7 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
@@ -1405,7 +1476,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1423,7 +1494,7 @@
         <v>34</v>
       </c>
       <c r="M15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1437,7 +1508,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>
@@ -1467,7 +1538,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1478,7 +1549,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
@@ -1505,10 +1576,10 @@
         <v>34</v>
       </c>
       <c r="M17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1519,7 +1590,7 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
@@ -1549,7 +1620,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1560,7 +1631,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
@@ -1590,7 +1661,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1601,7 +1672,7 @@
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
         <v>21</v>
@@ -1610,7 +1681,7 @@
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1628,10 +1699,10 @@
         <v>34</v>
       </c>
       <c r="M20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1642,7 +1713,7 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
         <v>21</v>
@@ -1672,7 +1743,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1683,7 +1754,7 @@
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
         <v>21</v>
@@ -1710,10 +1781,10 @@
         <v>34</v>
       </c>
       <c r="M22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1724,7 +1795,7 @@
         <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
         <v>21</v>
@@ -1754,7 +1825,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1765,7 +1836,7 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
         <v>21</v>
@@ -1795,7 +1866,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1806,7 +1877,7 @@
         <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
         <v>21</v>
@@ -1815,7 +1886,7 @@
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1833,21 +1904,21 @@
         <v>34</v>
       </c>
       <c r="M25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" t="s">
-        <v>106</v>
       </c>
       <c r="E26" t="s">
         <v>21</v>
@@ -1877,7 +1948,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1888,7 +1959,7 @@
         <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
         <v>21</v>
@@ -1915,10 +1986,10 @@
         <v>34</v>
       </c>
       <c r="M27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1929,7 +2000,7 @@
         <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E28" t="s">
         <v>22</v>
@@ -1950,16 +2021,19 @@
         <v>1989</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="L28" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M28" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1970,7 +2044,7 @@
         <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E29" t="s">
         <v>22</v>
@@ -1991,16 +2065,19 @@
         <v>1989</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="L29" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2011,7 +2088,7 @@
         <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
         <v>22</v>
@@ -2020,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -2032,16 +2109,19 @@
         <v>1989</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="L30" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="N30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2052,7 +2132,7 @@
         <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
         <v>22</v>
@@ -2073,16 +2153,19 @@
         <v>1989</v>
       </c>
       <c r="K31">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="L31" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M31" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2093,7 +2176,7 @@
         <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E32" t="s">
         <v>22</v>
@@ -2114,16 +2197,19 @@
         <v>1989</v>
       </c>
       <c r="K32">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="L32" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M32" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="N32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2134,7 +2220,7 @@
         <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E33" t="s">
         <v>57</v>
@@ -2154,17 +2240,20 @@
       <c r="J33">
         <v>1989</v>
       </c>
-      <c r="K33" s="5">
-        <v>1</v>
+      <c r="K33">
+        <v>1000</v>
       </c>
       <c r="L33" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="N33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2175,7 +2264,7 @@
         <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E34" t="s">
         <v>57</v>
@@ -2195,17 +2284,20 @@
       <c r="J34">
         <v>1989</v>
       </c>
-      <c r="K34" s="5">
-        <v>1</v>
+      <c r="K34">
+        <v>1000</v>
       </c>
       <c r="L34" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="N34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2216,7 +2308,7 @@
         <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
         <v>57</v>
@@ -2225,7 +2317,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2236,28 +2328,31 @@
       <c r="J35">
         <v>1989</v>
       </c>
-      <c r="K35" s="5">
-        <v>1</v>
+      <c r="K35">
+        <v>1000</v>
       </c>
       <c r="L35" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M35" t="s">
+        <v>113</v>
+      </c>
+      <c r="N35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" t="s">
-        <v>107</v>
       </c>
       <c r="E36" t="s">
         <v>57</v>
@@ -2277,17 +2372,20 @@
       <c r="J36">
         <v>1989</v>
       </c>
-      <c r="K36" s="5">
-        <v>1</v>
+      <c r="K36">
+        <v>1000</v>
       </c>
       <c r="L36" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="N36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2298,7 +2396,7 @@
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E37" t="s">
         <v>57</v>
@@ -2318,17 +2416,20 @@
       <c r="J37">
         <v>1989</v>
       </c>
-      <c r="K37" s="5">
-        <v>1</v>
+      <c r="K37">
+        <v>1000</v>
       </c>
       <c r="L37" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M37" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="N37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2339,7 +2440,7 @@
         <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E38" t="s">
         <v>57</v>
@@ -2359,17 +2460,20 @@
       <c r="J38">
         <v>1989</v>
       </c>
-      <c r="K38" s="5">
-        <v>1</v>
+      <c r="K38">
+        <v>1000</v>
       </c>
       <c r="L38" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="N38" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -2380,7 +2484,7 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E39" t="s">
         <v>57</v>
@@ -2400,17 +2504,20 @@
       <c r="J39">
         <v>1989</v>
       </c>
-      <c r="K39" s="5">
-        <v>1</v>
+      <c r="K39">
+        <v>1000</v>
       </c>
       <c r="L39" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="N39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -2421,7 +2528,7 @@
         <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
         <v>57</v>
@@ -2430,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2441,17 +2548,20 @@
       <c r="J40">
         <v>1989</v>
       </c>
-      <c r="K40" s="5">
-        <v>1</v>
+      <c r="K40">
+        <v>1000</v>
       </c>
       <c r="L40" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="N40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2462,7 +2572,7 @@
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E41" t="s">
         <v>57</v>
@@ -2482,17 +2592,20 @@
       <c r="J41">
         <v>1989</v>
       </c>
-      <c r="K41" s="5">
-        <v>1</v>
+      <c r="K41">
+        <v>1000</v>
       </c>
       <c r="L41" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="N41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2503,7 +2616,7 @@
         <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E42" t="s">
         <v>57</v>
@@ -2523,17 +2636,20 @@
       <c r="J42">
         <v>1989</v>
       </c>
-      <c r="K42" s="5">
-        <v>1</v>
+      <c r="K42">
+        <v>1000</v>
       </c>
       <c r="L42" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="N42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2544,7 +2660,7 @@
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E43" t="s">
         <v>57</v>
@@ -2564,17 +2680,20 @@
       <c r="J43">
         <v>1989</v>
       </c>
-      <c r="K43" s="5">
-        <v>1</v>
+      <c r="K43">
+        <v>1000</v>
       </c>
       <c r="L43" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="N43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -2585,7 +2704,7 @@
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
         <v>57</v>
@@ -2605,17 +2724,20 @@
       <c r="J44">
         <v>1989</v>
       </c>
-      <c r="K44" s="5">
-        <v>1</v>
+      <c r="K44">
+        <v>1000</v>
       </c>
       <c r="L44" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M44" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="N44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -2626,7 +2748,7 @@
         <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
         <v>57</v>
@@ -2635,7 +2757,7 @@
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -2646,17 +2768,20 @@
       <c r="J45">
         <v>1989</v>
       </c>
-      <c r="K45" s="5">
-        <v>1</v>
+      <c r="K45">
+        <v>1000</v>
       </c>
       <c r="L45" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="N45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -2667,7 +2792,7 @@
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E46" t="s">
         <v>57</v>
@@ -2687,17 +2812,20 @@
       <c r="J46">
         <v>1989</v>
       </c>
-      <c r="K46" s="5">
-        <v>1</v>
+      <c r="K46">
+        <v>1000</v>
       </c>
       <c r="L46" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="N46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -2708,7 +2836,7 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E47" t="s">
         <v>57</v>
@@ -2728,17 +2856,20 @@
       <c r="J47">
         <v>1989</v>
       </c>
-      <c r="K47" s="5">
-        <v>1</v>
+      <c r="K47">
+        <v>1000</v>
       </c>
       <c r="L47" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="N47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -2749,7 +2880,7 @@
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E48" t="s">
         <v>57</v>
@@ -2769,14 +2900,17 @@
       <c r="J48">
         <v>1989</v>
       </c>
-      <c r="K48" s="5">
-        <v>1</v>
+      <c r="K48">
+        <v>1000</v>
       </c>
       <c r="L48" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M48" t="s">
-        <v>82</v>
+        <v>126</v>
+      </c>
+      <c r="N48" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -2790,7 +2924,7 @@
         <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E49" t="s">
         <v>57</v>
@@ -2810,14 +2944,17 @@
       <c r="J49">
         <v>1989</v>
       </c>
-      <c r="K49" s="5">
-        <v>1</v>
+      <c r="K49">
+        <v>1000</v>
       </c>
       <c r="L49" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M49" t="s">
-        <v>80</v>
+        <v>127</v>
+      </c>
+      <c r="N49" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -2831,7 +2968,7 @@
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
         <v>57</v>
@@ -2840,7 +2977,7 @@
         <v>4</v>
       </c>
       <c r="G50" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -2851,14 +2988,17 @@
       <c r="J50">
         <v>1989</v>
       </c>
-      <c r="K50" s="5">
-        <v>1</v>
+      <c r="K50">
+        <v>1000</v>
       </c>
       <c r="L50" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M50" t="s">
-        <v>90</v>
+        <v>128</v>
+      </c>
+      <c r="N50" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -2872,7 +3012,7 @@
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E51" t="s">
         <v>57</v>
@@ -2892,14 +3032,17 @@
       <c r="J51">
         <v>1989</v>
       </c>
-      <c r="K51" s="5">
-        <v>1</v>
+      <c r="K51">
+        <v>1000</v>
       </c>
       <c r="L51" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M51" t="s">
-        <v>81</v>
+        <v>129</v>
+      </c>
+      <c r="N51" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -2913,7 +3056,7 @@
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E52" t="s">
         <v>57</v>
@@ -2933,14 +3076,17 @@
       <c r="J52">
         <v>1989</v>
       </c>
-      <c r="K52" s="5">
-        <v>1</v>
+      <c r="K52">
+        <v>1000</v>
       </c>
       <c r="L52" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M52" t="s">
-        <v>98</v>
+        <v>130</v>
+      </c>
+      <c r="N52" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -2954,7 +3100,7 @@
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E53" t="s">
         <v>57</v>
@@ -2974,14 +3120,17 @@
       <c r="J53">
         <v>1989</v>
       </c>
-      <c r="K53" s="5">
-        <v>1</v>
+      <c r="K53">
+        <v>1000</v>
       </c>
       <c r="L53" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M53" t="s">
-        <v>82</v>
+        <v>135</v>
+      </c>
+      <c r="N53" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -2995,7 +3144,7 @@
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E54" t="s">
         <v>57</v>
@@ -3015,14 +3164,17 @@
       <c r="J54">
         <v>1989</v>
       </c>
-      <c r="K54" s="5">
-        <v>1</v>
+      <c r="K54">
+        <v>1000</v>
       </c>
       <c r="L54" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M54" t="s">
-        <v>80</v>
+        <v>131</v>
+      </c>
+      <c r="N54" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -3036,7 +3188,7 @@
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E55" t="s">
         <v>57</v>
@@ -3045,7 +3197,7 @@
         <v>5</v>
       </c>
       <c r="G55" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3056,14 +3208,17 @@
       <c r="J55">
         <v>1989</v>
       </c>
-      <c r="K55" s="5">
-        <v>1</v>
+      <c r="K55">
+        <v>1000</v>
       </c>
       <c r="L55" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M55" t="s">
-        <v>90</v>
+        <v>132</v>
+      </c>
+      <c r="N55" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -3077,7 +3232,7 @@
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E56" t="s">
         <v>57</v>
@@ -3097,14 +3252,17 @@
       <c r="J56">
         <v>1989</v>
       </c>
-      <c r="K56" s="5">
-        <v>1</v>
+      <c r="K56">
+        <v>1000</v>
       </c>
       <c r="L56" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M56" t="s">
-        <v>81</v>
+        <v>133</v>
+      </c>
+      <c r="N56" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -3118,7 +3276,7 @@
         <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E57" t="s">
         <v>57</v>
@@ -3138,14 +3296,17 @@
       <c r="J57">
         <v>1989</v>
       </c>
-      <c r="K57" s="5">
-        <v>1</v>
+      <c r="K57">
+        <v>1000</v>
       </c>
       <c r="L57" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M57" t="s">
-        <v>98</v>
+        <v>134</v>
+      </c>
+      <c r="N57" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -3159,7 +3320,7 @@
         <v>15</v>
       </c>
       <c r="D58" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E58" t="s">
         <v>57</v>
@@ -3179,14 +3340,17 @@
       <c r="J58">
         <v>1989</v>
       </c>
-      <c r="K58" s="5">
-        <v>1</v>
+      <c r="K58">
+        <v>1000</v>
       </c>
       <c r="L58" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M58" t="s">
-        <v>82</v>
+        <v>136</v>
+      </c>
+      <c r="N58" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -3200,7 +3364,7 @@
         <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E59" t="s">
         <v>57</v>
@@ -3220,14 +3384,17 @@
       <c r="J59">
         <v>1989</v>
       </c>
-      <c r="K59" s="5">
-        <v>1</v>
+      <c r="K59">
+        <v>1000</v>
       </c>
       <c r="L59" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M59" t="s">
-        <v>80</v>
+        <v>137</v>
+      </c>
+      <c r="N59" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -3241,7 +3408,7 @@
         <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E60" t="s">
         <v>57</v>
@@ -3250,7 +3417,7 @@
         <v>6</v>
       </c>
       <c r="G60" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -3261,14 +3428,17 @@
       <c r="J60">
         <v>1989</v>
       </c>
-      <c r="K60" s="5">
-        <v>1</v>
+      <c r="K60">
+        <v>1000</v>
       </c>
       <c r="L60" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M60" t="s">
-        <v>90</v>
+        <v>138</v>
+      </c>
+      <c r="N60" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -3282,7 +3452,7 @@
         <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E61" t="s">
         <v>57</v>
@@ -3302,14 +3472,17 @@
       <c r="J61">
         <v>1989</v>
       </c>
-      <c r="K61" s="5">
-        <v>1</v>
+      <c r="K61">
+        <v>1000</v>
       </c>
       <c r="L61" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M61" t="s">
-        <v>81</v>
+        <v>139</v>
+      </c>
+      <c r="N61" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -3323,7 +3496,7 @@
         <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="E62" t="s">
         <v>57</v>
@@ -3343,37 +3516,40 @@
       <c r="J62">
         <v>1989</v>
       </c>
-      <c r="K62" s="5">
-        <v>1</v>
+      <c r="K62">
+        <v>1000</v>
       </c>
       <c r="L62" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="M62" t="s">
-        <v>98</v>
+        <v>140</v>
+      </c>
+      <c r="N62" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="D63" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="E63" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -3391,7 +3567,7 @@
         <v>2</v>
       </c>
       <c r="M63" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -3408,7 +3584,7 @@
         <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -3455,7 +3631,7 @@
         <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -3499,7 +3675,7 @@
         <v>9</v>
       </c>
       <c r="E66" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="F66">
         <v>1</v>

</xml_diff>

<commit_message>
Character "NA" in `env` now blank
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="152">
   <si>
     <t>plant stress</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>mm</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>helps with coastal shrubland</t>
@@ -865,7 +862,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,93 +886,85 @@
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
         <v>79</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>80</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>81</v>
       </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>82</v>
-      </c>
       <c r="H2">
         <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
       </c>
       <c r="K2">
         <v>1000</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="L2" s="5"/>
       <c r="M2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" t="s">
         <v>84</v>
-      </c>
-      <c r="O2" t="s">
-        <v>85</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="2"/>
@@ -983,34 +972,28 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>80</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>81</v>
       </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>82</v>
-      </c>
       <c r="H3">
         <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>5</v>
       </c>
       <c r="K3">
         <v>10000</v>
@@ -1019,10 +1002,10 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="2"/>
@@ -1030,35 +1013,30 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J4" s="7"/>
       <c r="K4">
         <v>1000</v>
       </c>
@@ -1066,10 +1044,10 @@
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="2"/>
@@ -1077,35 +1055,30 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J5" s="7"/>
       <c r="K5">
         <v>1</v>
       </c>
@@ -1113,85 +1086,75 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J6" s="7"/>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J7" s="7"/>
       <c r="K7">
         <v>1</v>
       </c>
@@ -1199,43 +1162,38 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J8" s="7"/>
       <c r="K8">
         <v>1</v>
       </c>
@@ -1243,169 +1201,149 @@
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J9" s="7"/>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J10" s="7"/>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J11" s="7"/>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J12" s="7"/>
       <c r="K12">
         <v>1</v>
       </c>
@@ -1413,39 +1351,39 @@
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13">
         <v>1989</v>
@@ -1454,39 +1392,39 @@
         <v>-100</v>
       </c>
       <c r="L13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J14">
         <v>1989</v>
@@ -1495,39 +1433,39 @@
         <v>-100</v>
       </c>
       <c r="L14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J15">
         <v>1989</v>
@@ -1536,39 +1474,39 @@
         <v>-100</v>
       </c>
       <c r="L15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J16">
         <v>1989</v>
@@ -1577,39 +1515,39 @@
         <v>-100</v>
       </c>
       <c r="L16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17">
         <v>1989</v>
@@ -1618,39 +1556,39 @@
         <v>-100</v>
       </c>
       <c r="L17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J18">
         <v>1989</v>
@@ -1659,39 +1597,39 @@
         <v>-100</v>
       </c>
       <c r="L18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J19">
         <v>1989</v>
@@ -1700,39 +1638,39 @@
         <v>-100</v>
       </c>
       <c r="L19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J20">
         <v>1989</v>
@@ -1741,39 +1679,39 @@
         <v>-100</v>
       </c>
       <c r="L20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J21">
         <v>1989</v>
@@ -1782,39 +1720,39 @@
         <v>-100</v>
       </c>
       <c r="L21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J22">
         <v>1989</v>
@@ -1823,39 +1761,39 @@
         <v>-100</v>
       </c>
       <c r="L22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23">
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J23">
         <v>1989</v>
@@ -1864,39 +1802,39 @@
         <v>-100</v>
       </c>
       <c r="L23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24">
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J24">
         <v>1989</v>
@@ -1905,39 +1843,39 @@
         <v>-100</v>
       </c>
       <c r="L24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25">
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J25">
         <v>1989</v>
@@ -1946,39 +1884,39 @@
         <v>-100</v>
       </c>
       <c r="L25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F26">
         <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J26">
         <v>1989</v>
@@ -1987,39 +1925,39 @@
         <v>-100</v>
       </c>
       <c r="L26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27">
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J27">
         <v>1989</v>
@@ -2028,39 +1966,39 @@
         <v>-100</v>
       </c>
       <c r="L27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J28">
         <v>1989</v>
@@ -2069,42 +2007,42 @@
         <v>1000</v>
       </c>
       <c r="L28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J29">
         <v>1989</v>
@@ -2113,42 +2051,42 @@
         <v>1000</v>
       </c>
       <c r="L29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J30">
         <v>1989</v>
@@ -2157,42 +2095,42 @@
         <v>1000</v>
       </c>
       <c r="L30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J31">
         <v>1989</v>
@@ -2201,42 +2139,42 @@
         <v>1000</v>
       </c>
       <c r="L31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J32">
         <v>1989</v>
@@ -2245,42 +2183,42 @@
         <v>1000</v>
       </c>
       <c r="L32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J33">
         <v>1989</v>
@@ -2289,42 +2227,42 @@
         <v>1000</v>
       </c>
       <c r="L33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
         <v>50</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>51</v>
-      </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J34">
         <v>1989</v>
@@ -2333,42 +2271,42 @@
         <v>1000</v>
       </c>
       <c r="L34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J35">
         <v>1989</v>
@@ -2377,42 +2315,42 @@
         <v>1000</v>
       </c>
       <c r="L35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J36">
         <v>1989</v>
@@ -2421,42 +2359,42 @@
         <v>1000</v>
       </c>
       <c r="L36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J37">
         <v>1989</v>
@@ -2465,42 +2403,42 @@
         <v>1000</v>
       </c>
       <c r="L37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J38">
         <v>1989</v>
@@ -2509,42 +2447,42 @@
         <v>1000</v>
       </c>
       <c r="L38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F39">
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J39">
         <v>1989</v>
@@ -2553,42 +2491,42 @@
         <v>1000</v>
       </c>
       <c r="L39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F40">
         <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J40">
         <v>1989</v>
@@ -2597,42 +2535,42 @@
         <v>1000</v>
       </c>
       <c r="L40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F41">
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J41">
         <v>1989</v>
@@ -2641,42 +2579,42 @@
         <v>1000</v>
       </c>
       <c r="L41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F42">
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J42">
         <v>1989</v>
@@ -2685,42 +2623,42 @@
         <v>1000</v>
       </c>
       <c r="L42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F43">
         <v>3</v>
       </c>
       <c r="G43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J43">
         <v>1989</v>
@@ -2729,42 +2667,42 @@
         <v>1000</v>
       </c>
       <c r="L43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F44">
         <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J44">
         <v>1989</v>
@@ -2773,42 +2711,42 @@
         <v>1000</v>
       </c>
       <c r="L44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F45">
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J45">
         <v>1989</v>
@@ -2817,42 +2755,42 @@
         <v>1000</v>
       </c>
       <c r="L45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F46">
         <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J46">
         <v>1989</v>
@@ -2861,42 +2799,42 @@
         <v>1000</v>
       </c>
       <c r="L46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F47">
         <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H47">
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J47">
         <v>1989</v>
@@ -2905,42 +2843,42 @@
         <v>1000</v>
       </c>
       <c r="L47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F48">
         <v>4</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J48">
         <v>1989</v>
@@ -2949,42 +2887,42 @@
         <v>1000</v>
       </c>
       <c r="L48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F49">
         <v>4</v>
       </c>
       <c r="G49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J49">
         <v>1989</v>
@@ -2993,42 +2931,42 @@
         <v>1000</v>
       </c>
       <c r="L49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F50">
         <v>4</v>
       </c>
       <c r="G50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J50">
         <v>1989</v>
@@ -3037,42 +2975,42 @@
         <v>1000</v>
       </c>
       <c r="L50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51">
         <v>4</v>
       </c>
       <c r="G51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J51">
         <v>1989</v>
@@ -3081,42 +3019,42 @@
         <v>1000</v>
       </c>
       <c r="L51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F52">
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H52">
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J52">
         <v>1989</v>
@@ -3125,42 +3063,42 @@
         <v>1000</v>
       </c>
       <c r="L52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F53">
         <v>5</v>
       </c>
       <c r="G53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H53">
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J53">
         <v>1989</v>
@@ -3169,42 +3107,42 @@
         <v>1000</v>
       </c>
       <c r="L53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F54">
         <v>5</v>
       </c>
       <c r="G54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J54">
         <v>1989</v>
@@ -3213,42 +3151,42 @@
         <v>1000</v>
       </c>
       <c r="L54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F55">
         <v>5</v>
       </c>
       <c r="G55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J55">
         <v>1989</v>
@@ -3257,42 +3195,42 @@
         <v>1000</v>
       </c>
       <c r="L55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F56">
         <v>5</v>
       </c>
       <c r="G56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J56">
         <v>1989</v>
@@ -3301,42 +3239,42 @@
         <v>1000</v>
       </c>
       <c r="L56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F57">
         <v>5</v>
       </c>
       <c r="G57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J57">
         <v>1989</v>
@@ -3345,42 +3283,42 @@
         <v>1000</v>
       </c>
       <c r="L57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F58">
         <v>6</v>
       </c>
       <c r="G58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J58">
         <v>1989</v>
@@ -3389,42 +3327,42 @@
         <v>1000</v>
       </c>
       <c r="L58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F59">
         <v>6</v>
       </c>
       <c r="G59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H59">
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J59">
         <v>1989</v>
@@ -3433,42 +3371,42 @@
         <v>1000</v>
       </c>
       <c r="L59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F60">
         <v>6</v>
       </c>
       <c r="G60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H60">
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J60">
         <v>1989</v>
@@ -3477,42 +3415,42 @@
         <v>1000</v>
       </c>
       <c r="L60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F61">
         <v>6</v>
       </c>
       <c r="G61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J61">
         <v>1989</v>
@@ -3521,42 +3459,42 @@
         <v>1000</v>
       </c>
       <c r="L61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M61" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F62">
         <v>6</v>
       </c>
       <c r="G62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H62">
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J62">
         <v>1989</v>
@@ -3565,42 +3503,42 @@
         <v>1000</v>
       </c>
       <c r="L62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N62" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" t="s">
         <v>87</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
+        <v>150</v>
+      </c>
+      <c r="E63" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
         <v>88</v>
       </c>
-      <c r="D63" t="s">
-        <v>151</v>
-      </c>
-      <c r="E63" t="s">
-        <v>90</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="G63" t="s">
-        <v>89</v>
-      </c>
       <c r="H63">
         <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J63">
         <v>1987</v>
@@ -3609,39 +3547,39 @@
         <v>10000</v>
       </c>
       <c r="L63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M63" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F64">
         <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H64">
         <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J64" s="7">
         <v>1950</v>
@@ -3653,10 +3591,10 @@
         <v>2</v>
       </c>
       <c r="M64" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O64" t="s">
         <v>0</v>
@@ -3664,31 +3602,31 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F65">
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H65">
         <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J65" s="7">
         <v>1950</v>
@@ -3700,7 +3638,7 @@
         <v>4</v>
       </c>
       <c r="M65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O65" t="s">
         <v>1</v>
@@ -3708,31 +3646,31 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F66">
         <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H66">
         <v>1</v>
       </c>
       <c r="I66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J66" s="7">
         <v>1950</v>
@@ -3741,10 +3679,10 @@
         <v>10</v>
       </c>
       <c r="L66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O66" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Ensuring match between `env` `data_name` and a url
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -514,10 +514,10 @@
     <t>non-green cover</t>
   </si>
   <si>
-    <t>fractional cover</t>
-  </si>
-  <si>
     <t>surface reflectance</t>
+  </si>
+  <si>
+    <t>persistent green</t>
   </si>
 </sst>
 </file>
@@ -870,8 +870,8 @@
   <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,7 +1992,7 @@
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E28" t="s">
         <v>20</v>
@@ -2036,7 +2036,7 @@
         <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
@@ -2080,7 +2080,7 @@
         <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E30" t="s">
         <v>20</v>
@@ -2124,7 +2124,7 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E31" t="s">
         <v>20</v>
@@ -2168,7 +2168,7 @@
         <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
@@ -2212,7 +2212,7 @@
         <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E33" t="s">
         <v>49</v>
@@ -2256,7 +2256,7 @@
         <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E34" t="s">
         <v>49</v>
@@ -2300,7 +2300,7 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E35" t="s">
         <v>49</v>
@@ -2344,7 +2344,7 @@
         <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E36" t="s">
         <v>49</v>
@@ -2388,7 +2388,7 @@
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E37" t="s">
         <v>49</v>
@@ -2432,7 +2432,7 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
         <v>49</v>
@@ -2476,7 +2476,7 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E39" t="s">
         <v>49</v>
@@ -2520,7 +2520,7 @@
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
         <v>49</v>
@@ -2564,7 +2564,7 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E41" t="s">
         <v>49</v>
@@ -2608,7 +2608,7 @@
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E42" t="s">
         <v>49</v>
@@ -2652,7 +2652,7 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E43" t="s">
         <v>49</v>
@@ -2696,7 +2696,7 @@
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E44" t="s">
         <v>49</v>
@@ -2740,7 +2740,7 @@
         <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E45" t="s">
         <v>49</v>
@@ -2784,7 +2784,7 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E46" t="s">
         <v>49</v>
@@ -2828,7 +2828,7 @@
         <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E47" t="s">
         <v>49</v>
@@ -2872,7 +2872,7 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" t="s">
         <v>49</v>
@@ -2916,7 +2916,7 @@
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E49" t="s">
         <v>49</v>
@@ -2960,7 +2960,7 @@
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" t="s">
         <v>49</v>
@@ -3004,7 +3004,7 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E51" t="s">
         <v>49</v>
@@ -3048,7 +3048,7 @@
         <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E52" t="s">
         <v>49</v>
@@ -3092,7 +3092,7 @@
         <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E53" t="s">
         <v>49</v>
@@ -3136,7 +3136,7 @@
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E54" t="s">
         <v>49</v>
@@ -3180,7 +3180,7 @@
         <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E55" t="s">
         <v>49</v>
@@ -3224,7 +3224,7 @@
         <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E56" t="s">
         <v>49</v>
@@ -3268,7 +3268,7 @@
         <v>13</v>
       </c>
       <c r="D57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E57" t="s">
         <v>49</v>
@@ -3312,7 +3312,7 @@
         <v>13</v>
       </c>
       <c r="D58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E58" t="s">
         <v>49</v>
@@ -3356,7 +3356,7 @@
         <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E59" t="s">
         <v>49</v>
@@ -3400,7 +3400,7 @@
         <v>13</v>
       </c>
       <c r="D60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E60" t="s">
         <v>49</v>
@@ -3444,7 +3444,7 @@
         <v>13</v>
       </c>
       <c r="D61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E61" t="s">
         <v>49</v>
@@ -3488,7 +3488,7 @@
         <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E62" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
persitent green cover transform and units fixed
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -870,8 +870,8 @@
   <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,11 +2012,11 @@
       <c r="J28">
         <v>1989</v>
       </c>
-      <c r="K28">
-        <v>1000</v>
+      <c r="K28" s="5">
+        <v>-100</v>
       </c>
       <c r="L28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M28" t="s">
         <v>53</v>
@@ -2056,11 +2056,11 @@
       <c r="J29">
         <v>1989</v>
       </c>
-      <c r="K29">
-        <v>1000</v>
+      <c r="K29" s="5">
+        <v>-100</v>
       </c>
       <c r="L29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M29" t="s">
         <v>51</v>
@@ -2100,11 +2100,11 @@
       <c r="J30">
         <v>1989</v>
       </c>
-      <c r="K30">
-        <v>1000</v>
+      <c r="K30" s="5">
+        <v>-100</v>
       </c>
       <c r="L30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M30" t="s">
         <v>63</v>
@@ -2144,11 +2144,11 @@
       <c r="J31">
         <v>1989</v>
       </c>
-      <c r="K31">
-        <v>1000</v>
+      <c r="K31" s="5">
+        <v>-100</v>
       </c>
       <c r="L31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M31" t="s">
         <v>52</v>
@@ -2188,11 +2188,11 @@
       <c r="J32">
         <v>1989</v>
       </c>
-      <c r="K32">
-        <v>1000</v>
+      <c r="K32" s="5">
+        <v>-100</v>
       </c>
       <c r="L32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M32" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
added indices to `env`
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="167">
   <si>
     <t>plant stress</t>
   </si>
@@ -519,12 +519,48 @@
   <si>
     <t>persistent green</t>
   </si>
+  <si>
+    <t>normalised difference vegetation index</t>
+  </si>
+  <si>
+    <t>ndvi</t>
+  </si>
+  <si>
+    <t>(nir - red) / (nir + red)</t>
+  </si>
+  <si>
+    <t>photosynthetic activity</t>
+  </si>
+  <si>
+    <t>ndmi</t>
+  </si>
+  <si>
+    <t>normalised difference moisture index</t>
+  </si>
+  <si>
+    <t>(nir - swir1) / (nir + swir1)</t>
+  </si>
+  <si>
+    <t>vegetation water content</t>
+  </si>
+  <si>
+    <t>msavi</t>
+  </si>
+  <si>
+    <t>modified soil adjusted vegetation index</t>
+  </si>
+  <si>
+    <t>(2 * nir + 1 - sqrt((2 * nir + 1)^2 - 8 * (nir - red)))/2</t>
+  </si>
+  <si>
+    <t>minimizes the effect of bare soil on the Soil Adjusted Vegetation Index (SAVI)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,14 +572,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -572,11 +600,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -585,10 +612,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -867,11 +892,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S67"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,7 +3723,145 @@
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D67" s="8"/>
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" t="s">
+        <v>153</v>
+      </c>
+      <c r="E67" t="s">
+        <v>156</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67" t="s">
+        <v>50</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" t="s">
+        <v>31</v>
+      </c>
+      <c r="J67" s="7">
+        <v>1989</v>
+      </c>
+      <c r="K67">
+        <v>10000</v>
+      </c>
+      <c r="L67" t="s">
+        <v>2</v>
+      </c>
+      <c r="M67" t="s">
+        <v>155</v>
+      </c>
+      <c r="N67" t="s">
+        <v>157</v>
+      </c>
+      <c r="O67" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" t="s">
+        <v>153</v>
+      </c>
+      <c r="E68" t="s">
+        <v>159</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68" t="s">
+        <v>50</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" t="s">
+        <v>31</v>
+      </c>
+      <c r="J68" s="7">
+        <v>1989</v>
+      </c>
+      <c r="K68">
+        <v>10000</v>
+      </c>
+      <c r="L68" t="s">
+        <v>2</v>
+      </c>
+      <c r="M68" t="s">
+        <v>160</v>
+      </c>
+      <c r="N68" t="s">
+        <v>161</v>
+      </c>
+      <c r="O68" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" t="s">
+        <v>153</v>
+      </c>
+      <c r="E69" t="s">
+        <v>163</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69" t="s">
+        <v>50</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
+        <v>31</v>
+      </c>
+      <c r="J69" s="7">
+        <v>1989</v>
+      </c>
+      <c r="K69">
+        <v>10000</v>
+      </c>
+      <c r="L69" t="s">
+        <v>2</v>
+      </c>
+      <c r="M69" t="s">
+        <v>164</v>
+      </c>
+      <c r="N69" t="s">
+        <v>165</v>
+      </c>
+      <c r="O69" t="s">
+        <v>166</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:O66">

</xml_diff>

<commit_message>
added `msavi` and `nbr2` to `env`
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="175">
   <si>
     <t>plant stress</t>
   </si>
@@ -554,6 +554,30 @@
   </si>
   <si>
     <t>minimizes the effect of bare soil on the Soil Adjusted Vegetation Index (SAVI)</t>
+  </si>
+  <si>
+    <t>nbr2</t>
+  </si>
+  <si>
+    <t>(nir - swir1)/(nir + swir1)</t>
+  </si>
+  <si>
+    <t>modifies the Normalized Burn Ratio (NBR) to highlight water sensitivity in vegetation and may be useful in post-fire recovery studies</t>
+  </si>
+  <si>
+    <t>normalised burn ratio 2</t>
+  </si>
+  <si>
+    <t>savi</t>
+  </si>
+  <si>
+    <t>soil adjusted vegetation index</t>
+  </si>
+  <si>
+    <t>((nir - red)/(nir + red + L)) * (1 + L)</t>
+  </si>
+  <si>
+    <t>used to correct Normalized Difference Vegetation Index (NDVI) for the influence of soil brightness in areas where vegetative cover is low</t>
   </si>
 </sst>
 </file>
@@ -892,11 +916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S69"/>
+  <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3863,6 +3887,100 @@
         <v>166</v>
       </c>
     </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" t="s">
+        <v>153</v>
+      </c>
+      <c r="E70" t="s">
+        <v>167</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70" t="s">
+        <v>50</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>31</v>
+      </c>
+      <c r="J70" s="7">
+        <v>1989</v>
+      </c>
+      <c r="K70">
+        <v>10000</v>
+      </c>
+      <c r="L70" t="s">
+        <v>2</v>
+      </c>
+      <c r="M70" t="s">
+        <v>170</v>
+      </c>
+      <c r="N70" t="s">
+        <v>168</v>
+      </c>
+      <c r="O70" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" t="s">
+        <v>153</v>
+      </c>
+      <c r="E71" t="s">
+        <v>171</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71" t="s">
+        <v>50</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" t="s">
+        <v>31</v>
+      </c>
+      <c r="J71" s="7">
+        <v>1989</v>
+      </c>
+      <c r="K71">
+        <v>10000</v>
+      </c>
+      <c r="L71" t="s">
+        <v>2</v>
+      </c>
+      <c r="M71" t="s">
+        <v>172</v>
+      </c>
+      <c r="N71" t="s">
+        <v>173</v>
+      </c>
+      <c r="O71" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:O66">
     <sortCondition ref="D2:D66"/>

</xml_diff>

<commit_message>
Added extra pasture classes
</commit_message>
<xml_diff>
--- a/data-raw/env.xlsx
+++ b/data-raw/env.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="176">
   <si>
     <t>plant stress</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>used to correct Normalized Difference Vegetation Index (NDVI) for the influence of soil brightness in areas where vegetative cover is low</t>
+  </si>
+  <si>
+    <t>indices</t>
   </si>
 </sst>
 </file>
@@ -919,8 +922,8 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3757,7 +3760,7 @@
         <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E67" t="s">
         <v>156</v>
@@ -3804,7 +3807,7 @@
         <v>13</v>
       </c>
       <c r="D68" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E68" t="s">
         <v>159</v>
@@ -3851,7 +3854,7 @@
         <v>13</v>
       </c>
       <c r="D69" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E69" t="s">
         <v>163</v>
@@ -3898,7 +3901,7 @@
         <v>13</v>
       </c>
       <c r="D70" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E70" t="s">
         <v>167</v>
@@ -3945,7 +3948,7 @@
         <v>13</v>
       </c>
       <c r="D71" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E71" t="s">
         <v>171</v>

</xml_diff>